<commit_message>
Finished extracting player data, next step is rank data
</commit_message>
<xml_diff>
--- a/table_format.xlsx
+++ b/table_format.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="players" sheetId="1" r:id="rId1"/>
-    <sheet name="game_types" sheetId="2" r:id="rId2"/>
+    <sheet name="rank" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -426,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>